<commit_message>
feat: Rename column name into english when preprocess.
</commit_message>
<xml_diff>
--- a/data/preprocess/pre-processed.xlsx
+++ b/data/preprocess/pre-processed.xlsx
@@ -436,57 +436,57 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>地块编号</t>
+          <t>Field ID</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>作物编号</t>
+          <t>Crop ID</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>作物名称</t>
+          <t>Crop Name</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>作物类型</t>
+          <t>Crop Type</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>种植面积/亩</t>
+          <t>Planting Area</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>种植季次</t>
+          <t>Season</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>地块类型</t>
+          <t>Field Type</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>地块面积/亩</t>
+          <t>Field Area</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>亩产量/斤</t>
+          <t>Yield</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>种植成本/(元/亩)</t>
+          <t>Cost</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>销售单价/(元/斤)</t>
+          <t>Price</t>
         </is>
       </c>
     </row>

</xml_diff>